<commit_message>
Fix Label Formating Loop - Increased Upload/Export WEB Timeout
</commit_message>
<xml_diff>
--- a/SessionBackup/LastSessionItems.xlsx
+++ b/SessionBackup/LastSessionItems.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27628"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ivan\Desktop\codebarPrintingTool\SessionBackup\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C342716E-D7FA-43EE-B038-2905BAB4EE4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0329C630-B235-45D9-94C9-37BA4BF3B10D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>

</xml_diff>

<commit_message>
Try fetching windows printer state and inquirer prompt
</commit_message>
<xml_diff>
--- a/SessionBackup/LastSessionItems.xlsx
+++ b/SessionBackup/LastSessionItems.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ivan\Desktop\barcodeUtils\SessionBackup\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ivan\Desktop\barcodeutils\SessionBackup\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0F9EDF1-2717-4961-A247-CA95F3CA87C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1A81F74-C9D0-4E12-9FBE-4A17943DC5FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4290" yWindow="4290" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Productos" sheetId="1" r:id="rId1"/>

</xml_diff>